<commit_message>
labs on template import
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32860" yWindow="3740" windowWidth="34160" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="0" windowWidth="34160" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Basic Model Designation</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Only used when pump cannot be tested at 120% BEP</t>
+  </si>
+  <si>
+    <t>Please enter Laboratory Certificate Number, or Name exactly as it is shown in the ER Portal</t>
   </si>
 </sst>
 </file>
@@ -1426,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1645,7 +1648,9 @@
       <c r="AK2" s="72"/>
       <c r="AL2" s="72"/>
       <c r="AM2" s="80"/>
-      <c r="AN2" s="83"/>
+      <c r="AN2" s="83" t="s">
+        <v>59</v>
+      </c>
       <c r="AO2" s="58" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
units of measure on import/export
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="0" windowWidth="34160" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="1060" windowWidth="34160" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -372,6 +372,17 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -689,7 +700,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -771,46 +782,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -818,88 +833,85 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -908,13 +920,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -923,13 +935,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -938,18 +953,15 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -957,59 +969,122 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1050,6 +1125,8 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1090,6 +1167,8 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1427,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO48"/>
+  <dimension ref="A1:AO49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AN3" sqref="AN3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1714,40 +1793,83 @@
       <c r="AN3" s="84"/>
       <c r="AO3" s="46"/>
     </row>
-    <row r="4" spans="1:41">
-      <c r="AM4" s="81"/>
+    <row r="4" spans="1:41" s="104" customFormat="1" ht="23" customHeight="1">
+      <c r="A4" s="85"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="93"/>
+      <c r="X4" s="93"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96"/>
+      <c r="AC4" s="96"/>
+      <c r="AD4" s="97"/>
+      <c r="AE4" s="98"/>
+      <c r="AF4" s="99"/>
+      <c r="AG4" s="99"/>
+      <c r="AH4" s="99"/>
+      <c r="AI4" s="100"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="93"/>
+      <c r="AL4" s="93"/>
+      <c r="AM4" s="101"/>
+      <c r="AN4" s="102"/>
+      <c r="AO4" s="103"/>
     </row>
-    <row r="8" spans="1:41">
-      <c r="AL8" s="1" t="s">
+    <row r="5" spans="1:41">
+      <c r="AM5" s="81"/>
+    </row>
+    <row r="9" spans="1:41">
+      <c r="AL9" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="5:5">
-      <c r="E32" s="19"/>
     </row>
     <row r="33" spans="5:5">
       <c r="E33" s="19"/>
     </row>
-    <row r="36" spans="5:5">
-      <c r="E36" s="19"/>
+    <row r="34" spans="5:5">
+      <c r="E34" s="19"/>
     </row>
     <row r="37" spans="5:5">
       <c r="E37" s="19"/>
     </row>
-    <row r="40" spans="5:5">
-      <c r="E40" s="19"/>
+    <row r="38" spans="5:5">
+      <c r="E38" s="19"/>
     </row>
     <row r="41" spans="5:5">
       <c r="E41" s="19"/>
     </row>
-    <row r="44" spans="5:5">
-      <c r="E44" s="19"/>
+    <row r="42" spans="5:5">
+      <c r="E42" s="19"/>
     </row>
     <row r="45" spans="5:5">
       <c r="E45" s="19"/>
     </row>
-    <row r="48" spans="5:5">
-      <c r="E48" s="19"/>
+    <row r="46" spans="5:5">
+      <c r="E46" s="19"/>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1770,7 +1892,7 @@
           <x14:formula1>
             <xm:f>Choicelists!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F4:F577</xm:sqref>
+          <xm:sqref>F5:F578</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
template export on calculator
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="1060" windowWidth="34160" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="30160" yWindow="340" windowWidth="34160" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -700,100 +710,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -807,77 +817,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -887,204 +840,281 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="5" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="14" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="3" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="88">
+    <cellStyle name="Comma" xfId="85" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1127,6 +1157,7 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1169,6 +1200,7 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1509,379 +1541,380 @@
   <dimension ref="A1:AO49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="11" style="1"/>
+    <col min="7" max="7" width="11" style="29"/>
+    <col min="8" max="9" width="11" style="1"/>
     <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
     <col min="11" max="12" width="11" style="1"/>
     <col min="13" max="13" width="19.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="11" style="3" customWidth="1"/>
-    <col min="17" max="18" width="11" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11" style="1"/>
-    <col min="20" max="20" width="11" style="4" customWidth="1"/>
-    <col min="21" max="21" width="11" style="1"/>
-    <col min="22" max="22" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="11" style="3"/>
-    <col min="27" max="27" width="11" style="62"/>
-    <col min="28" max="28" width="11" style="2"/>
-    <col min="29" max="29" width="11" style="1"/>
-    <col min="30" max="30" width="11" style="4"/>
-    <col min="31" max="31" width="11" style="3"/>
-    <col min="32" max="33" width="11" style="1"/>
-    <col min="34" max="34" width="11" style="4"/>
-    <col min="35" max="35" width="11" style="3"/>
-    <col min="36" max="36" width="11" style="3" customWidth="1"/>
-    <col min="37" max="38" width="11" style="1" customWidth="1"/>
-    <col min="39" max="39" width="11" style="4" customWidth="1"/>
-    <col min="40" max="40" width="21.33203125" style="6" customWidth="1"/>
-    <col min="41" max="41" width="18.6640625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="11" style="43" customWidth="1"/>
+    <col min="17" max="18" width="11" style="44" customWidth="1"/>
+    <col min="19" max="19" width="11" style="44"/>
+    <col min="20" max="20" width="11" style="45" customWidth="1"/>
+    <col min="21" max="21" width="11" style="44"/>
+    <col min="22" max="22" width="0" style="43" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="0" style="44" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="0" style="108" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="0" style="109" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="43"/>
+    <col min="27" max="27" width="11" style="110"/>
+    <col min="28" max="28" width="11" style="108"/>
+    <col min="29" max="29" width="11" style="44"/>
+    <col min="30" max="30" width="11" style="45"/>
+    <col min="31" max="31" width="11" style="43"/>
+    <col min="32" max="33" width="11" style="44"/>
+    <col min="34" max="34" width="11" style="45"/>
+    <col min="35" max="35" width="11" style="43"/>
+    <col min="36" max="36" width="11" style="43" customWidth="1"/>
+    <col min="37" max="38" width="11" style="44" customWidth="1"/>
+    <col min="39" max="39" width="11" style="45" customWidth="1"/>
+    <col min="40" max="40" width="21.33203125" style="112" customWidth="1"/>
+    <col min="41" max="41" width="18.6640625" style="112" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="18" customFormat="1" ht="142.5" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:41" s="8" customFormat="1" ht="142.5" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="T1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="61" t="s">
+      <c r="Z1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AA1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AB1" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="60" t="s">
+      <c r="AC1" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" s="29" t="s">
+      <c r="AD1" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AE1" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AG1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="17" t="s">
+      <c r="AH1" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" s="68" t="s">
+      <c r="AI1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="73" t="s">
+      <c r="AJ1" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AK1" s="74" t="s">
+      <c r="AK1" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" s="74" t="s">
+      <c r="AL1" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="71" t="s">
+      <c r="AM1" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="AN1" s="82" t="s">
+      <c r="AN1" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" s="22" t="s">
+      <c r="AO1" s="63" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="36" customFormat="1" ht="99" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="59" t="s">
+    <row r="2" spans="1:41" s="14" customFormat="1" ht="99" customHeight="1">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31" t="s">
+      <c r="N2" s="12"/>
+      <c r="O2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="48" t="s">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="64"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="50"/>
-      <c r="AE2" s="53" t="s">
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="79"/>
-      <c r="AK2" s="72"/>
-      <c r="AL2" s="72"/>
-      <c r="AM2" s="80"/>
-      <c r="AN2" s="83" t="s">
+      <c r="AF2" s="72"/>
+      <c r="AG2" s="72"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="74"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="76"/>
+      <c r="AL2" s="76"/>
+      <c r="AM2" s="77"/>
+      <c r="AN2" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="AO2" s="58" t="s">
+      <c r="AO2" s="79" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="47" customFormat="1" ht="83" customHeight="1" thickBot="1">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="40" t="s">
+    <row r="3" spans="1:41" s="19" customFormat="1" ht="83" customHeight="1" thickBot="1">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="43" t="s">
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="44" t="s">
+      <c r="W3" s="81"/>
+      <c r="X3" s="81"/>
+      <c r="Y3" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="56" t="s">
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="AB3" s="57"/>
-      <c r="AC3" s="56" t="s">
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="AD3" s="52"/>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="70"/>
-      <c r="AJ3" s="75" t="s">
+      <c r="AD3" s="86"/>
+      <c r="AE3" s="87"/>
+      <c r="AF3" s="87"/>
+      <c r="AG3" s="87"/>
+      <c r="AH3" s="87"/>
+      <c r="AI3" s="88"/>
+      <c r="AJ3" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="AK3" s="78"/>
-      <c r="AL3" s="76" t="s">
+      <c r="AK3" s="90"/>
+      <c r="AL3" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="AM3" s="77"/>
-      <c r="AN3" s="84"/>
-      <c r="AO3" s="46"/>
+      <c r="AM3" s="92"/>
+      <c r="AN3" s="93"/>
+      <c r="AO3" s="94"/>
     </row>
-    <row r="4" spans="1:41" s="104" customFormat="1" ht="23" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="95"/>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="96"/>
-      <c r="AC4" s="96"/>
-      <c r="AD4" s="97"/>
-      <c r="AE4" s="98"/>
-      <c r="AF4" s="99"/>
-      <c r="AG4" s="99"/>
-      <c r="AH4" s="99"/>
-      <c r="AI4" s="100"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="93"/>
-      <c r="AL4" s="93"/>
-      <c r="AM4" s="101"/>
-      <c r="AN4" s="102"/>
-      <c r="AO4" s="103"/>
+    <row r="4" spans="1:41" s="24" customFormat="1" ht="23" customHeight="1">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="96"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="97"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="100"/>
+      <c r="AC4" s="100"/>
+      <c r="AD4" s="101"/>
+      <c r="AE4" s="102"/>
+      <c r="AF4" s="103"/>
+      <c r="AG4" s="103"/>
+      <c r="AH4" s="103"/>
+      <c r="AI4" s="104"/>
+      <c r="AJ4" s="96"/>
+      <c r="AK4" s="97"/>
+      <c r="AL4" s="97"/>
+      <c r="AM4" s="105"/>
+      <c r="AN4" s="106"/>
+      <c r="AO4" s="107"/>
     </row>
     <row r="5" spans="1:41">
-      <c r="AM5" s="81"/>
+      <c r="AM5" s="111"/>
     </row>
     <row r="9" spans="1:41">
-      <c r="AL9" s="1" t="s">
+      <c r="AL9" s="44" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="19"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="5:5">
-      <c r="E34" s="19"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="19"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" spans="5:5">
-      <c r="E38" s="19"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="41" spans="5:5">
-      <c r="E41" s="19"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" spans="5:5">
-      <c r="E42" s="19"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="45" spans="5:5">
-      <c r="E45" s="19"/>
+      <c r="E45" s="9"/>
     </row>
     <row r="46" spans="5:5">
-      <c r="E46" s="19"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="49" spans="5:5">
-      <c r="E49" s="19"/>
+      <c r="E49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="AE3:AH3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="AJ3:AK3"/>
     <mergeCell ref="AL3:AM3"/>
     <mergeCell ref="Z2:AD2"/>
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="AE3:AH3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="AJ3:AK3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1914,28 +1947,27 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="10" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
help links in template
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -25,9 +25,6 @@
     <t>Basic Model Designation</t>
   </si>
   <si>
-    <t>Impeller Diameter</t>
-  </si>
-  <si>
     <t>Nominal Speed</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
   </si>
   <si>
     <t>Brand name</t>
-  </si>
-  <si>
-    <t>Equipment Class of rated pump</t>
   </si>
   <si>
     <t>Bare pump</t>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t>Please enter Laboratory Certificate Number, or Name exactly as it is shown in the ER Portal</t>
+  </si>
+  <si>
+    <t>Equipment Category of rated pump</t>
+  </si>
+  <si>
+    <t>"Full" Impeller Diameter</t>
   </si>
 </sst>
 </file>
@@ -213,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -265,20 +265,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -710,7 +696,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -799,32 +785,18 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -864,9 +836,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="5" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -877,18 +846,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -897,15 +854,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -919,57 +867,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -985,24 +882,6 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1022,9 +901,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1033,31 +909,7 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1112,8 +964,140 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="88" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="88" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="88" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="5" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="88" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="88" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="10" borderId="7" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="11" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="7" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="13" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="5" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="2" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="7" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="1" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="5" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="7" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="26" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="27" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="25" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="13" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="11" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="89">
     <cellStyle name="Comma" xfId="85" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1201,6 +1185,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1540,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1551,373 +1536,414 @@
     <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="29"/>
+    <col min="7" max="7" width="11" style="23"/>
     <col min="8" max="9" width="11" style="1"/>
     <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
     <col min="11" max="12" width="11" style="1"/>
     <col min="13" max="13" width="19.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.83203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11" style="43" customWidth="1"/>
-    <col min="17" max="18" width="11" style="44" customWidth="1"/>
-    <col min="19" max="19" width="11" style="44"/>
-    <col min="20" max="20" width="11" style="45" customWidth="1"/>
-    <col min="21" max="21" width="11" style="44"/>
-    <col min="22" max="22" width="0" style="43" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="0" style="44" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="0" style="108" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="0" style="109" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="11" style="43"/>
-    <col min="27" max="27" width="11" style="110"/>
-    <col min="28" max="28" width="11" style="108"/>
-    <col min="29" max="29" width="11" style="44"/>
-    <col min="30" max="30" width="11" style="45"/>
-    <col min="31" max="31" width="11" style="43"/>
-    <col min="32" max="33" width="11" style="44"/>
-    <col min="34" max="34" width="11" style="45"/>
-    <col min="35" max="35" width="11" style="43"/>
-    <col min="36" max="36" width="11" style="43" customWidth="1"/>
-    <col min="37" max="38" width="11" style="44" customWidth="1"/>
-    <col min="39" max="39" width="11" style="45" customWidth="1"/>
-    <col min="40" max="40" width="21.33203125" style="112" customWidth="1"/>
-    <col min="41" max="41" width="18.6640625" style="112" customWidth="1"/>
+    <col min="16" max="16" width="11" style="30" customWidth="1"/>
+    <col min="17" max="18" width="11" style="31" customWidth="1"/>
+    <col min="19" max="19" width="11" style="31"/>
+    <col min="20" max="20" width="11" style="32" customWidth="1"/>
+    <col min="21" max="21" width="11" style="31"/>
+    <col min="22" max="22" width="0" style="30" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="0" style="31" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="0" style="63" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="0" style="64" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="30"/>
+    <col min="27" max="27" width="11" style="65"/>
+    <col min="28" max="28" width="11" style="63"/>
+    <col min="29" max="29" width="11" style="31"/>
+    <col min="30" max="30" width="11" style="32"/>
+    <col min="31" max="31" width="11" style="30"/>
+    <col min="32" max="33" width="11" style="31"/>
+    <col min="34" max="34" width="11" style="32"/>
+    <col min="35" max="35" width="11" style="30"/>
+    <col min="36" max="36" width="11" style="30" customWidth="1"/>
+    <col min="37" max="38" width="11" style="31" customWidth="1"/>
+    <col min="39" max="39" width="11" style="32" customWidth="1"/>
+    <col min="40" max="40" width="21.33203125" style="67" customWidth="1"/>
+    <col min="41" max="41" width="18.6640625" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="8" customFormat="1" ht="142.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:41" s="4" customFormat="1" ht="142.5" customHeight="1">
+      <c r="A1" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="88" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="88" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="O1" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="92" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="X1" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="100" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB1" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="102" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="103" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="104" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF1" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG1" s="105" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH1" s="106" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI1" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ1" s="107" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="108" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="108" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM1" s="109" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN1" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="AO1" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" s="9" customFormat="1" ht="99" customHeight="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="79"/>
+      <c r="AE2" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y1" s="49" t="s">
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="85"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="40"/>
+      <c r="AL2" s="40"/>
+      <c r="AM2" s="41"/>
+      <c r="AN2" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO2" s="43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" s="14" customFormat="1" ht="83" customHeight="1" thickBot="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA1" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB1" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC1" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD1" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE1" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF1" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG1" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH1" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI1" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ1" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK1" s="60" t="s">
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM1" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN1" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="AO1" s="63" t="s">
-        <v>21</v>
-      </c>
+      <c r="AB3" s="82"/>
+      <c r="AC3" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD3" s="81"/>
+      <c r="AE3" s="69"/>
+      <c r="AF3" s="69"/>
+      <c r="AG3" s="69"/>
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="47"/>
+      <c r="AJ3" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK3" s="74"/>
+      <c r="AL3" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM3" s="76"/>
+      <c r="AN3" s="48"/>
+      <c r="AO3" s="49"/>
     </row>
-    <row r="2" spans="1:41" s="14" customFormat="1" ht="99" customHeight="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="72"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="76"/>
-      <c r="AL2" s="76"/>
-      <c r="AM2" s="77"/>
-      <c r="AN2" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO2" s="79" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" s="19" customFormat="1" ht="83" customHeight="1" thickBot="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="80"/>
-      <c r="V3" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="W3" s="81"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="82" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB3" s="85"/>
-      <c r="AC3" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD3" s="86"/>
-      <c r="AE3" s="87"/>
-      <c r="AF3" s="87"/>
-      <c r="AG3" s="87"/>
-      <c r="AH3" s="87"/>
-      <c r="AI3" s="88"/>
-      <c r="AJ3" s="89" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK3" s="90"/>
-      <c r="AL3" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM3" s="92"/>
-      <c r="AN3" s="93"/>
-      <c r="AO3" s="94"/>
-    </row>
-    <row r="4" spans="1:41" s="24" customFormat="1" ht="23" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="95"/>
-      <c r="V4" s="96"/>
-      <c r="W4" s="97"/>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="98"/>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="100"/>
-      <c r="AB4" s="100"/>
-      <c r="AC4" s="100"/>
-      <c r="AD4" s="101"/>
-      <c r="AE4" s="102"/>
-      <c r="AF4" s="103"/>
-      <c r="AG4" s="103"/>
-      <c r="AH4" s="103"/>
-      <c r="AI4" s="104"/>
-      <c r="AJ4" s="96"/>
-      <c r="AK4" s="97"/>
-      <c r="AL4" s="97"/>
-      <c r="AM4" s="105"/>
-      <c r="AN4" s="106"/>
-      <c r="AO4" s="107"/>
+    <row r="4" spans="1:41" s="19" customFormat="1" ht="23" customHeight="1">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="52"/>
+      <c r="Y4" s="53"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="55"/>
+      <c r="AB4" s="55"/>
+      <c r="AC4" s="55"/>
+      <c r="AD4" s="56"/>
+      <c r="AE4" s="57"/>
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="51"/>
+      <c r="AK4" s="52"/>
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="60"/>
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="62"/>
     </row>
     <row r="5" spans="1:41">
-      <c r="AM5" s="111"/>
+      <c r="AM5" s="66"/>
     </row>
     <row r="9" spans="1:41">
-      <c r="AL9" s="44" t="s">
-        <v>49</v>
+      <c r="AL9" s="31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="9"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="5:5">
-      <c r="E34" s="9"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="9"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="5:5">
-      <c r="E38" s="9"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="41" spans="5:5">
-      <c r="E41" s="9"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="5:5">
-      <c r="E42" s="9"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="45" spans="5:5">
-      <c r="E45" s="9"/>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" spans="5:5">
-      <c r="E46" s="9"/>
+      <c r="E46" s="5"/>
     </row>
     <row r="49" spans="5:5">
-      <c r="E49" s="9"/>
+      <c r="E49" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AE2:AH2"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="P3:T3"/>
     <mergeCell ref="AJ3:AK3"/>
     <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AE2:AH2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="participant"/>
+    <hyperlink ref="B1" r:id="rId2" location="brand"/>
+    <hyperlink ref="C1" r:id="rId3" location="basic_model_number"/>
+    <hyperlink ref="D1" r:id="rId4" location="individual_model_number"/>
+    <hyperlink ref="E1" r:id="rId5" location="category"/>
+    <hyperlink ref="F1" r:id="rId6" location="configuration"/>
+    <hyperlink ref="G1" r:id="rId7" location="diameter"/>
+    <hyperlink ref="H1" r:id="rId8" location="section"/>
+    <hyperlink ref="I1" r:id="rId9" location="stages"/>
+    <hyperlink ref="J1" r:id="rId10" location="speed"/>
+    <hyperlink ref="K1" r:id="rId11" location="bowl_diameter"/>
+    <hyperlink ref="L1" r:id="rId12" location="motor_regulated"/>
+    <hyperlink ref="M1" r:id="rId13" location="nominal_efficiency"/>
+    <hyperlink ref="N1" r:id="rId14" location="motor_power_rated_3"/>
+    <hyperlink ref="O1" r:id="rId15" location="bep120"/>
+    <hyperlink ref="P1" r:id="rId16" location="rep_nominal_speed"/>
+    <hyperlink ref="Q1" r:id="rId17" location="rep_nominal_speed"/>
+    <hyperlink ref="R1" r:id="rId18" location="rep_nominal_speed"/>
+    <hyperlink ref="S1" r:id="rId19" location="rep_nominal_speed"/>
+    <hyperlink ref="T1" r:id="rId20" location="rep_nominal_speed"/>
+    <hyperlink ref="U1" r:id="rId21" location="rep_nominal_speed"/>
+    <hyperlink ref="V1" r:id="rId22" location="rep_nominal_speed"/>
+    <hyperlink ref="W1" r:id="rId23" location="rep_nominal_speed"/>
+    <hyperlink ref="X1" r:id="rId24" location="rep_nominal_speed"/>
+    <hyperlink ref="Y1" r:id="rId25" location="rep_nominal_speed"/>
+    <hyperlink ref="Z1" r:id="rId26" location="rep_nominal_speed"/>
+    <hyperlink ref="AA1" r:id="rId27" location="rep_nominal_speed"/>
+    <hyperlink ref="AB1" r:id="rId28" location="rep_nominal_speed"/>
+    <hyperlink ref="AC1" r:id="rId29" location="rep_nominal_speed"/>
+    <hyperlink ref="AD1" r:id="rId30" location="rep_nominal_speed"/>
+    <hyperlink ref="AE1" r:id="rId31" location="rep_nominal_speed"/>
+    <hyperlink ref="AF1" r:id="rId32" location="rep_nominal_speed"/>
+    <hyperlink ref="AG1" r:id="rId33" location="rep_nominal_speed"/>
+    <hyperlink ref="AH1" r:id="rId34" location="rep_nominal_speed"/>
+    <hyperlink ref="AJ1" r:id="rId35" location="rep_nominal_speed"/>
+    <hyperlink ref="AK1" r:id="rId36" location="rep_nominal_speed"/>
+    <hyperlink ref="AL1" r:id="rId37" location="rep_nominal_speed"/>
+    <hyperlink ref="AM1" r:id="rId38" location="rep_nominal_speed"/>
+    <hyperlink ref="AI1" r:id="rId39" location="pei_entry"/>
+    <hyperlink ref="AN1" r:id="rId40" location="lab"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1947,23 +1973,23 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="10" t="s">
-        <v>29</v>
+      <c r="A1" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="10" t="s">
-        <v>30</v>
+      <c r="A2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="10" t="s">
-        <v>31</v>
+      <c r="A3" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="10" t="s">
-        <v>32</v>
+      <c r="A4" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pump listings export
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA810C0-8929-4AB4-AD88-366B66EA59D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37920" yWindow="1620" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Choicelists" sheetId="2" r:id="rId2"/>
     <sheet name="Version" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
-  <si>
-    <t>Basic Model Designation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Nominal Speed</t>
   </si>
@@ -89,18 +92,9 @@
     <t xml:space="preserve">Section of Appendix A to Subpart Y </t>
   </si>
   <si>
-    <t>Pump Bowl Diameter if applicable</t>
-  </si>
-  <si>
-    <t>Manufacturer (individual) model number</t>
-  </si>
-  <si>
     <t>HI Laboratory #</t>
   </si>
   <si>
-    <t>Configuration of rated pump</t>
-  </si>
-  <si>
     <t>Brand name</t>
   </si>
   <si>
@@ -114,15 +108,6 @@
   </si>
   <si>
     <t>Bare pump + motor + non-continuous control</t>
-  </si>
-  <si>
-    <t>Participant / Manufacturer</t>
-  </si>
-  <si>
-    <t>For RSV and ST Pumps # of Stages</t>
-  </si>
-  <si>
-    <t>For section III, the Motor power used for default losses or for section IV, V, VI, VII, the   rated motor horsepower</t>
   </si>
   <si>
     <t>Bare pump
@@ -192,9 +177,6 @@
     <t>Equipment Category of rated pump</t>
   </si>
   <si>
-    <t>"Full" Impeller Diameter</t>
-  </si>
-  <si>
     <t>3600 or 1800</t>
   </si>
   <si>
@@ -230,13 +212,46 @@
   <si>
     <t>Revision Date</t>
   </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Basic Model Number</t>
+  </si>
+  <si>
+    <t>Individual Model Number</t>
+  </si>
+  <si>
+    <t>Pump Configuration</t>
+  </si>
+  <si>
+    <t>Full Impeller Diameter</t>
+  </si>
+  <si>
+    <t>For RSV and ST Pumps, the Number of Stages</t>
+  </si>
+  <si>
+    <t>For ST Pumps, the Bowl Diameter</t>
+  </si>
+  <si>
+    <t>For Section III, the Motor Power used for Default Losses or for Section IV, V, VI, VII, the Rated Motor</t>
+  </si>
+  <si>
+    <t>Pump Listing Status</t>
+  </si>
+  <si>
+    <t>Rating ID</t>
+  </si>
+  <si>
+    <t>Listing Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -293,7 +308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +369,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -807,12 +828,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -861,16 +882,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="14" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="3" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="85" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -989,7 +1010,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="88" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="5" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="88" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="88" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,6 +1158,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1565,28 +1595,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AR49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AR2" sqref="AR2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.33203125" style="96" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.375" style="96" customWidth="1"/>
+    <col min="5" max="5" width="21.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="23"/>
-    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.625" style="1" customWidth="1"/>
     <col min="11" max="12" width="11" style="1"/>
-    <col min="13" max="13" width="19.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="19.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.875" style="3" customWidth="1"/>
     <col min="16" max="16" width="11" style="30" customWidth="1"/>
     <col min="17" max="18" width="11" style="31" customWidth="1"/>
     <col min="19" max="19" width="11" style="31"/>
@@ -1608,164 +1638,173 @@
     <col min="36" max="36" width="11" style="30" customWidth="1"/>
     <col min="37" max="38" width="11" style="31" customWidth="1"/>
     <col min="39" max="39" width="11" style="32" customWidth="1"/>
-    <col min="40" max="40" width="21.33203125" style="64" customWidth="1"/>
-    <col min="41" max="41" width="18.6640625" style="64" customWidth="1"/>
+    <col min="40" max="40" width="21.375" style="64" customWidth="1"/>
+    <col min="41" max="44" width="18.625" style="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="4" customFormat="1" ht="142.5" customHeight="1">
+    <row r="1" spans="1:44" s="4" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="67" t="s">
+      <c r="T1" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF1" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG1" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH1" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI1" s="89" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ1" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL1" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM1" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN1" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="72" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" s="72" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" s="74" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="75" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" s="76" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="77" t="s">
-        <v>9</v>
-      </c>
-      <c r="X1" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" s="80" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB1" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="81" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE1" s="83" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF1" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG1" s="84" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH1" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI1" s="89" t="s">
+      <c r="AO1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="86" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK1" s="87" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL1" s="87" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM1" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN1" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="AO1" s="33" t="s">
-        <v>20</v>
+      <c r="AP1" s="120" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ1" s="120" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR1" s="120" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="9" customFormat="1" ht="99" customHeight="1">
+    <row r="2" spans="1:44" s="9" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="93"/>
       <c r="D2" s="93"/>
       <c r="E2" s="91" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="P2" s="24"/>
       <c r="Q2" s="25"/>
@@ -1773,40 +1812,49 @@
       <c r="S2" s="25"/>
       <c r="T2" s="26"/>
       <c r="U2" s="34" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="V2" s="35"/>
       <c r="W2" s="36"/>
       <c r="X2" s="36"/>
       <c r="Y2" s="37"/>
       <c r="Z2" s="109" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="AA2" s="110"/>
       <c r="AB2" s="110"/>
       <c r="AC2" s="110"/>
       <c r="AD2" s="111"/>
       <c r="AE2" s="115" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="AF2" s="116"/>
       <c r="AG2" s="116"/>
       <c r="AH2" s="117"/>
       <c r="AI2" s="38"/>
       <c r="AJ2" s="106" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AK2" s="107"/>
       <c r="AL2" s="107"/>
       <c r="AM2" s="108"/>
       <c r="AN2" s="39" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AO2" s="40" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="AP2" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ2" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR2" s="121" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="14" customFormat="1" ht="83" customHeight="1" thickBot="1">
+    <row r="3" spans="1:44" s="14" customFormat="1" ht="83.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="94"/>
@@ -1822,10 +1870,10 @@
       <c r="M3" s="12"/>
       <c r="N3" s="11"/>
       <c r="O3" s="13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="P3" s="99" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="100"/>
       <c r="R3" s="100"/>
@@ -1833,20 +1881,20 @@
       <c r="T3" s="101"/>
       <c r="U3" s="41"/>
       <c r="V3" s="118" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W3" s="118"/>
       <c r="X3" s="118"/>
       <c r="Y3" s="42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z3" s="43"/>
       <c r="AA3" s="112" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AB3" s="114"/>
       <c r="AC3" s="112" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="AD3" s="113"/>
       <c r="AE3" s="119"/>
@@ -1855,17 +1903,20 @@
       <c r="AH3" s="119"/>
       <c r="AI3" s="44"/>
       <c r="AJ3" s="102" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AK3" s="103"/>
       <c r="AL3" s="104" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="AM3" s="105"/>
       <c r="AN3" s="45"/>
       <c r="AO3" s="46"/>
+      <c r="AP3" s="122"/>
+      <c r="AQ3" s="122"/>
+      <c r="AR3" s="122"/>
     </row>
-    <row r="4" spans="1:41" s="19" customFormat="1" ht="23" customHeight="1">
+    <row r="4" spans="1:44" s="19" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="95"/>
@@ -1907,40 +1958,43 @@
       <c r="AM4" s="57"/>
       <c r="AN4" s="58"/>
       <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59"/>
+      <c r="AR4" s="59"/>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AM5" s="63"/>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AL9" s="31" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="33" spans="5:5">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="5"/>
     </row>
-    <row r="37" spans="5:5">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="5:5">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" s="5"/>
     </row>
-    <row r="41" spans="5:5">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="5:5">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E42" s="5"/>
     </row>
-    <row r="45" spans="5:5">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="5:5">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E46" s="5"/>
     </row>
-    <row r="49" spans="5:5">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49" s="5"/>
     </row>
   </sheetData>
@@ -1957,52 +2011,52 @@
     <mergeCell ref="AE3:AH3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="participant"/>
-    <hyperlink ref="B1" r:id="rId2" location="brand"/>
-    <hyperlink ref="C1" r:id="rId3" location="basic_model_number"/>
-    <hyperlink ref="D1" r:id="rId4" location="individual_model_number"/>
-    <hyperlink ref="E1" r:id="rId5" location="category"/>
-    <hyperlink ref="F1" r:id="rId6" location="configuration"/>
-    <hyperlink ref="G1" r:id="rId7" location="diameter"/>
-    <hyperlink ref="H1" r:id="rId8" location="section"/>
-    <hyperlink ref="I1" r:id="rId9" location="stages"/>
-    <hyperlink ref="J1" r:id="rId10" location="speed"/>
-    <hyperlink ref="K1" r:id="rId11" location="bowl_diameter"/>
-    <hyperlink ref="L1" r:id="rId12" location="motor_regulated"/>
-    <hyperlink ref="M1" r:id="rId13" location="nominal_efficiency"/>
-    <hyperlink ref="N1" r:id="rId14" location="motor_power_rated_3"/>
-    <hyperlink ref="O1" r:id="rId15" location="bep120"/>
-    <hyperlink ref="P1" r:id="rId16" location="rep_nominal_speed"/>
-    <hyperlink ref="Q1" r:id="rId17" location="rep_nominal_speed"/>
-    <hyperlink ref="R1" r:id="rId18" location="rep_nominal_speed"/>
-    <hyperlink ref="S1" r:id="rId19" location="rep_nominal_speed"/>
-    <hyperlink ref="T1" r:id="rId20" location="rep_nominal_speed"/>
-    <hyperlink ref="U1" r:id="rId21" location="rep_nominal_speed"/>
-    <hyperlink ref="V1" r:id="rId22" location="rep_nominal_speed"/>
-    <hyperlink ref="W1" r:id="rId23" location="rep_nominal_speed"/>
-    <hyperlink ref="X1" r:id="rId24" location="rep_nominal_speed"/>
-    <hyperlink ref="Y1" r:id="rId25" location="rep_nominal_speed"/>
-    <hyperlink ref="Z1" r:id="rId26" location="rep_nominal_speed"/>
-    <hyperlink ref="AA1" r:id="rId27" location="rep_nominal_speed"/>
-    <hyperlink ref="AB1" r:id="rId28" location="rep_nominal_speed"/>
-    <hyperlink ref="AC1" r:id="rId29" location="rep_nominal_speed"/>
-    <hyperlink ref="AD1" r:id="rId30" location="rep_nominal_speed"/>
-    <hyperlink ref="AE1" r:id="rId31" location="rep_nominal_speed"/>
-    <hyperlink ref="AF1" r:id="rId32" location="rep_nominal_speed"/>
-    <hyperlink ref="AG1" r:id="rId33" location="rep_nominal_speed"/>
-    <hyperlink ref="AH1" r:id="rId34" location="rep_nominal_speed"/>
-    <hyperlink ref="AJ1" r:id="rId35" location="rep_nominal_speed"/>
-    <hyperlink ref="AK1" r:id="rId36" location="rep_nominal_speed"/>
-    <hyperlink ref="AL1" r:id="rId37" location="rep_nominal_speed"/>
-    <hyperlink ref="AM1" r:id="rId38" location="rep_nominal_speed"/>
-    <hyperlink ref="AI1" r:id="rId39" location="pei_entry"/>
-    <hyperlink ref="AN1" r:id="rId40" location="lab"/>
+    <hyperlink ref="A1" r:id="rId1" location="participant" display="Participant / Manufacturer" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId2" location="brand" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C1" r:id="rId3" location="basic_model_number" display="Basic Model Designation" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" location="individual_model_number" display="Manufacturer (individual) model number" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E1" r:id="rId5" location="category" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F1" r:id="rId6" location="configuration" display="Configuration of rated pump" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G1" r:id="rId7" location="diameter" display="&quot;Full&quot; Impeller Diameter" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H1" r:id="rId8" location="section" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I1" r:id="rId9" location="stages" display="For RSV and ST Pumps # of Stages" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J1" r:id="rId10" location="speed" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="K1" r:id="rId11" location="bowl_diameter" display="Pump Bowl Diameter if applicable" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="L1" r:id="rId12" location="motor_regulated" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="M1" r:id="rId13" location="nominal_efficiency" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="N1" r:id="rId14" location="motor_power_rated_3" display="For section III, the Motor power used for default losses or for section IV, V, VI, VII, the   rated motor horsepower" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="O1" r:id="rId15" location="bep120" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="P1" r:id="rId16" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="Q1" r:id="rId17" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="R1" r:id="rId18" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="S1" r:id="rId19" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="T1" r:id="rId20" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="U1" r:id="rId21" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="V1" r:id="rId22" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="W1" r:id="rId23" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="X1" r:id="rId24" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="Y1" r:id="rId25" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="Z1" r:id="rId26" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="AA1" r:id="rId27" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="AB1" r:id="rId28" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="AC1" r:id="rId29" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="AD1" r:id="rId30" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="AE1" r:id="rId31" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="AF1" r:id="rId32" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="AG1" r:id="rId33" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="AH1" r:id="rId34" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="AJ1" r:id="rId35" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="AK1" r:id="rId36" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="AL1" r:id="rId37" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="AM1" r:id="rId38" location="rep_nominal_speed" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="AI1" r:id="rId39" location="pei_entry" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="AN1" r:id="rId40" location="lab" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Choicelists!$A$1:$A$4</xm:f>
           </x14:formula1>
@@ -2018,33 +2072,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2058,29 +2112,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B1" s="97" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B2" s="98">
         <v>42767</v>

</xml_diff>

<commit_message>
Updated download file with savings columns
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hi-er\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33D76B9-BAB9-4640-AECC-A684001761D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62DE65E-7320-470A-B75B-B9DEC779800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="4500" windowWidth="26295" windowHeight="10980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>Nominal Speed</t>
   </si>
@@ -285,6 +285,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Annual Energy Savings</t>
+  </si>
+  <si>
+    <t>Annual Cost Savings</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -357,7 +369,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,8 +436,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -792,6 +810,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -884,7 +950,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1135,6 +1201,26 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1193,6 +1279,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1622,27 +1714,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AQ5" sqref="AQ5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="84" customWidth="1"/>
+    <col min="1" max="1" width="27.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.09765625" style="84" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="84" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="21"/>
-    <col min="8" max="8" width="13.375" customWidth="1"/>
-    <col min="10" max="10" width="11.625" customWidth="1"/>
-    <col min="12" max="12" width="34.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.375" customWidth="1"/>
-    <col min="15" max="15" width="18.375" customWidth="1"/>
-    <col min="16" max="16" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.3984375" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" customWidth="1"/>
+    <col min="12" max="12" width="34.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.3984375" customWidth="1"/>
+    <col min="15" max="15" width="18.3984375" customWidth="1"/>
+    <col min="16" max="16" width="14.8984375" style="2" customWidth="1"/>
     <col min="17" max="17" width="11" style="28" customWidth="1"/>
     <col min="18" max="19" width="11" style="29" customWidth="1"/>
     <col min="20" max="20" width="11" style="29"/>
@@ -1660,11 +1752,13 @@
     <col min="33" max="33" width="11" style="28" customWidth="1"/>
     <col min="34" max="35" width="11" style="29" customWidth="1"/>
     <col min="36" max="36" width="11" style="30" customWidth="1"/>
-    <col min="37" max="37" width="21.375" style="56" customWidth="1"/>
-    <col min="38" max="41" width="18.625" style="56" customWidth="1"/>
+    <col min="37" max="37" width="21.3984375" style="56" customWidth="1"/>
+    <col min="38" max="41" width="18.59765625" style="56" customWidth="1"/>
+    <col min="42" max="42" width="11" style="94"/>
+    <col min="43" max="43" width="11" style="95"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="3" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>49</v>
       </c>
@@ -1788,8 +1882,14 @@
       <c r="AO1" s="87" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" s="7" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="AP1" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ1" s="97" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" s="7" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -1838,26 +1938,26 @@
       <c r="V2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="104" t="s">
+      <c r="W2" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="105"/>
-      <c r="Y2" s="105"/>
-      <c r="Z2" s="105"/>
-      <c r="AA2" s="106"/>
-      <c r="AB2" s="110" t="s">
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="114"/>
+      <c r="AB2" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="112"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="119"/>
+      <c r="AE2" s="120"/>
       <c r="AF2" s="33"/>
-      <c r="AG2" s="101" t="s">
+      <c r="AG2" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="102"/>
-      <c r="AI2" s="102"/>
-      <c r="AJ2" s="103"/>
+      <c r="AH2" s="110"/>
+      <c r="AI2" s="110"/>
+      <c r="AJ2" s="111"/>
       <c r="AK2" s="34" t="s">
         <v>38</v>
       </c>
@@ -1873,8 +1973,14 @@
       <c r="AO2" s="88" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" s="12" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP2" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ2" s="99" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" s="12" customFormat="1" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="82"/>
@@ -1893,43 +1999,45 @@
       <c r="P3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="94" t="s">
+      <c r="Q3" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="96"/>
+      <c r="R3" s="103"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="103"/>
+      <c r="U3" s="104"/>
       <c r="V3" s="36"/>
       <c r="W3" s="37"/>
-      <c r="X3" s="107" t="s">
+      <c r="X3" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="107" t="s">
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="115" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="108"/>
-      <c r="AB3" s="113"/>
-      <c r="AC3" s="113"/>
-      <c r="AD3" s="113"/>
-      <c r="AE3" s="113"/>
+      <c r="AA3" s="116"/>
+      <c r="AB3" s="121"/>
+      <c r="AC3" s="121"/>
+      <c r="AD3" s="121"/>
+      <c r="AE3" s="121"/>
       <c r="AF3" s="38"/>
-      <c r="AG3" s="97" t="s">
+      <c r="AG3" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="98"/>
-      <c r="AI3" s="99" t="s">
+      <c r="AH3" s="106"/>
+      <c r="AI3" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="AJ3" s="100"/>
+      <c r="AJ3" s="108"/>
       <c r="AK3" s="39"/>
       <c r="AL3" s="40"/>
       <c r="AM3" s="89"/>
       <c r="AN3" s="89"/>
       <c r="AO3" s="89"/>
-    </row>
-    <row r="4" spans="1:41" s="17" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP3" s="100"/>
+      <c r="AQ3" s="101"/>
+    </row>
+    <row r="4" spans="1:43" s="17" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="83"/>
@@ -1971,11 +2079,17 @@
       <c r="AM4" s="89"/>
       <c r="AN4" s="89"/>
       <c r="AO4" s="89"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP4" s="122" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ4" s="123" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AJ5" s="55"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AI9" s="29" t="s">
         <v>28</v>
       </c>
@@ -2039,7 +2153,7 @@
           <x14:formula1>
             <xm:f>Choicelists!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F101:F578 F5:F100</xm:sqref>
+          <xm:sqref>F5:F578</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{368E6EB0-807F-47B8-8B52-718C2947B13F}">
           <x14:formula1>
@@ -2088,9 +2202,9 @@
       <selection activeCell="F15" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
         <v>52</v>
       </c>
@@ -2098,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2106,7 +2220,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2114,22 +2228,22 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" s="92" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="93" t="s">
         <v>60</v>
       </c>
@@ -2137,7 +2251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2145,7 +2259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2153,7 +2267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2161,22 +2275,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="92" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2184,7 +2298,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2192,7 +2306,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -2200,7 +2314,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -2223,12 +2337,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -2236,7 +2350,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Put ER Savings and Cost savings in common
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hi-er\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62DE65E-7320-470A-B75B-B9DEC779800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B5560B-A0EA-4B23-9A91-581B2DEB8352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4716" yWindow="3648" windowWidth="19860" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>Nominal Speed</t>
   </si>
@@ -291,12 +291,6 @@
   </si>
   <si>
     <t>Annual Cost Savings</t>
-  </si>
-  <si>
-    <t>kWh</t>
-  </si>
-  <si>
-    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -1221,6 +1215,12 @@
     <xf numFmtId="2" fontId="6" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1279,12 +1279,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1717,7 +1711,7 @@
   <dimension ref="A1:AQ9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AQ5" sqref="AQ5"/>
+      <selection activeCell="AQ4" sqref="AQ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1938,26 +1932,26 @@
       <c r="V2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="112" t="s">
+      <c r="W2" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
-      <c r="AA2" s="114"/>
-      <c r="AB2" s="118" t="s">
+      <c r="X2" s="115"/>
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="AC2" s="119"/>
-      <c r="AD2" s="119"/>
-      <c r="AE2" s="120"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="122"/>
       <c r="AF2" s="33"/>
-      <c r="AG2" s="109" t="s">
+      <c r="AG2" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="110"/>
-      <c r="AI2" s="110"/>
-      <c r="AJ2" s="111"/>
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="112"/>
+      <c r="AJ2" s="113"/>
       <c r="AK2" s="34" t="s">
         <v>38</v>
       </c>
@@ -1999,36 +1993,36 @@
       <c r="P3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="102" t="s">
+      <c r="Q3" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="103"/>
-      <c r="S3" s="103"/>
-      <c r="T3" s="103"/>
-      <c r="U3" s="104"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="106"/>
       <c r="V3" s="36"/>
       <c r="W3" s="37"/>
-      <c r="X3" s="115" t="s">
+      <c r="X3" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="115" t="s">
+      <c r="Y3" s="119"/>
+      <c r="Z3" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="116"/>
-      <c r="AB3" s="121"/>
-      <c r="AC3" s="121"/>
-      <c r="AD3" s="121"/>
-      <c r="AE3" s="121"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="123"/>
+      <c r="AC3" s="123"/>
+      <c r="AD3" s="123"/>
+      <c r="AE3" s="123"/>
       <c r="AF3" s="38"/>
-      <c r="AG3" s="105" t="s">
+      <c r="AG3" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="106"/>
-      <c r="AI3" s="107" t="s">
+      <c r="AH3" s="108"/>
+      <c r="AI3" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="AJ3" s="108"/>
+      <c r="AJ3" s="110"/>
       <c r="AK3" s="39"/>
       <c r="AL3" s="40"/>
       <c r="AM3" s="89"/>
@@ -2079,12 +2073,8 @@
       <c r="AM4" s="89"/>
       <c r="AN4" s="89"/>
       <c r="AO4" s="89"/>
-      <c r="AP4" s="122" t="s">
-        <v>81</v>
-      </c>
-      <c r="AQ4" s="123" t="s">
-        <v>82</v>
-      </c>
+      <c r="AP4" s="102"/>
+      <c r="AQ4" s="103"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AJ5" s="55"/>
@@ -2334,7 +2324,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2347,7 +2337,7 @@
         <v>47</v>
       </c>
       <c r="B1" s="85">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2355,7 +2345,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="86">
-        <v>45194</v>
+        <v>45391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
open to first line
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hi-er\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B5560B-A0EA-4B23-9A91-581B2DEB8352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CA52A0-ED1B-4F58-BF2C-7E3078C0BE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4716" yWindow="3648" windowWidth="19860" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1710,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AQ4" sqref="AQ4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
2024 02 22 label work (#1)
* Change Comsumptive to Efficient

* Added message at bottom of label

* Added blocks

* DISABLED EMAIL

* updated tag (small) label

* Change circulator labels back to Most/Least Consumptive

* Update pugs.

* Change default email push

* HE-7 Mods to Energy Labels

* update package.json-lock

* update label

* update

* Small label

* label working

* label_builder

* mod

* Revert

* include fonts.pug

* Helvetica only

* update

* more

* more

* test

* final

* empty lines

* small

* normal

* Updated download file with savings columns

* Put ER Savings and Cost savings in common

* open to first line

* Cleanup files
</commit_message>
<xml_diff>
--- a/routes/er_pump_listings.xlsx
+++ b/routes/er_pump_listings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hi-er\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33D76B9-BAB9-4640-AECC-A684001761D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CA52A0-ED1B-4F58-BF2C-7E3078C0BE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="4500" windowWidth="26295" windowHeight="10980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4716" yWindow="3648" windowWidth="19860" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>Nominal Speed</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Annual Energy Savings</t>
+  </si>
+  <si>
+    <t>Annual Cost Savings</t>
   </si>
 </sst>
 </file>
@@ -357,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,8 +430,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -792,6 +804,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -884,7 +944,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1135,6 +1195,32 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1622,27 +1708,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AQ9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="84" customWidth="1"/>
+    <col min="1" max="1" width="27.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.09765625" style="84" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="84" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="21"/>
-    <col min="8" max="8" width="13.375" customWidth="1"/>
-    <col min="10" max="10" width="11.625" customWidth="1"/>
-    <col min="12" max="12" width="34.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.375" customWidth="1"/>
-    <col min="15" max="15" width="18.375" customWidth="1"/>
-    <col min="16" max="16" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.3984375" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" customWidth="1"/>
+    <col min="12" max="12" width="34.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.3984375" customWidth="1"/>
+    <col min="15" max="15" width="18.3984375" customWidth="1"/>
+    <col min="16" max="16" width="14.8984375" style="2" customWidth="1"/>
     <col min="17" max="17" width="11" style="28" customWidth="1"/>
     <col min="18" max="19" width="11" style="29" customWidth="1"/>
     <col min="20" max="20" width="11" style="29"/>
@@ -1660,11 +1746,13 @@
     <col min="33" max="33" width="11" style="28" customWidth="1"/>
     <col min="34" max="35" width="11" style="29" customWidth="1"/>
     <col min="36" max="36" width="11" style="30" customWidth="1"/>
-    <col min="37" max="37" width="21.375" style="56" customWidth="1"/>
-    <col min="38" max="41" width="18.625" style="56" customWidth="1"/>
+    <col min="37" max="37" width="21.3984375" style="56" customWidth="1"/>
+    <col min="38" max="41" width="18.59765625" style="56" customWidth="1"/>
+    <col min="42" max="42" width="11" style="94"/>
+    <col min="43" max="43" width="11" style="95"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="3" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>49</v>
       </c>
@@ -1788,8 +1876,14 @@
       <c r="AO1" s="87" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" s="7" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="AP1" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ1" s="97" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" s="7" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -1838,26 +1932,26 @@
       <c r="V2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="104" t="s">
+      <c r="W2" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="105"/>
-      <c r="Y2" s="105"/>
-      <c r="Z2" s="105"/>
-      <c r="AA2" s="106"/>
-      <c r="AB2" s="110" t="s">
+      <c r="X2" s="115"/>
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="112"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="122"/>
       <c r="AF2" s="33"/>
-      <c r="AG2" s="101" t="s">
+      <c r="AG2" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="102"/>
-      <c r="AI2" s="102"/>
-      <c r="AJ2" s="103"/>
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="112"/>
+      <c r="AJ2" s="113"/>
       <c r="AK2" s="34" t="s">
         <v>38</v>
       </c>
@@ -1873,8 +1967,14 @@
       <c r="AO2" s="88" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" s="12" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP2" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ2" s="99" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" s="12" customFormat="1" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="82"/>
@@ -1893,43 +1993,45 @@
       <c r="P3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="94" t="s">
+      <c r="Q3" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="96"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="106"/>
       <c r="V3" s="36"/>
       <c r="W3" s="37"/>
-      <c r="X3" s="107" t="s">
+      <c r="X3" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="107" t="s">
+      <c r="Y3" s="119"/>
+      <c r="Z3" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="108"/>
-      <c r="AB3" s="113"/>
-      <c r="AC3" s="113"/>
-      <c r="AD3" s="113"/>
-      <c r="AE3" s="113"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="123"/>
+      <c r="AC3" s="123"/>
+      <c r="AD3" s="123"/>
+      <c r="AE3" s="123"/>
       <c r="AF3" s="38"/>
-      <c r="AG3" s="97" t="s">
+      <c r="AG3" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="98"/>
-      <c r="AI3" s="99" t="s">
+      <c r="AH3" s="108"/>
+      <c r="AI3" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="AJ3" s="100"/>
+      <c r="AJ3" s="110"/>
       <c r="AK3" s="39"/>
       <c r="AL3" s="40"/>
       <c r="AM3" s="89"/>
       <c r="AN3" s="89"/>
       <c r="AO3" s="89"/>
-    </row>
-    <row r="4" spans="1:41" s="17" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP3" s="100"/>
+      <c r="AQ3" s="101"/>
+    </row>
+    <row r="4" spans="1:43" s="17" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="83"/>
@@ -1971,11 +2073,13 @@
       <c r="AM4" s="89"/>
       <c r="AN4" s="89"/>
       <c r="AO4" s="89"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP4" s="102"/>
+      <c r="AQ4" s="103"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AJ5" s="55"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AI9" s="29" t="s">
         <v>28</v>
       </c>
@@ -2039,7 +2143,7 @@
           <x14:formula1>
             <xm:f>Choicelists!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F101:F578 F5:F100</xm:sqref>
+          <xm:sqref>F5:F578</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{368E6EB0-807F-47B8-8B52-718C2947B13F}">
           <x14:formula1>
@@ -2088,9 +2192,9 @@
       <selection activeCell="F15" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
         <v>52</v>
       </c>
@@ -2098,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2106,7 +2210,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2114,22 +2218,22 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" s="92" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="93" t="s">
         <v>60</v>
       </c>
@@ -2137,7 +2241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2145,7 +2249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2153,7 +2257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2161,22 +2265,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="92" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2184,7 +2288,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2192,7 +2296,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -2200,7 +2304,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -2220,28 +2324,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="85">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="86">
-        <v>45194</v>
+        <v>45391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>